<commit_message>
Filters and export fix - missing filtered output
</commit_message>
<xml_diff>
--- a/inst/extdata/filtersTemplate.xlsx
+++ b/inst/extdata/filtersTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annan\OneDrive\Desktop\OSMtidy V0.0.4\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\av57\Documents\GitHub\OSMtidy\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8917C721-9BDB-4FD9-9787-5A98522EC63B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9E5C19-19EA-42E7-A2BF-9AE725EE877C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E90EB3F-0E8A-4B2F-895F-8F54793F508B}"/>
+    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" xr2:uid="{2E90EB3F-0E8A-4B2F-895F-8F54793F508B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>searchColumn_contains</t>
   </si>
@@ -44,16 +44,7 @@
     <t>validate</t>
   </si>
   <si>
-    <t>name1</t>
-  </si>
-  <si>
-    <t>name2</t>
-  </si>
-  <si>
     <t>descTerm</t>
-  </si>
-  <si>
-    <t>description</t>
   </si>
 </sst>
 </file>
@@ -133,16 +124,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EAC31272-28D3-4C78-AD6B-57EF5A17AC2E}" name="Table1" displayName="Table1" ref="A1:G2" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:G2" xr:uid="{1DAAA34F-827B-442A-80BD-93609DE1A7AF}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EAC31272-28D3-4C78-AD6B-57EF5A17AC2E}" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:D2" xr:uid="{1DAAA34F-827B-442A-80BD-93609DE1A7AF}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A5B92B5E-072F-4EB8-AFDA-2F596212DBF6}" name="searchColumn_contains" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{0AB205AB-CA0B-495A-9296-8B5C34808190}" name="searchTerm" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{152AD9AE-64E4-482B-B971-B25B35A45187}" name="validate" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{13EB982F-1D9E-43D6-93E1-271A1140B8A4}" name="name1" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{C7686A2E-FE7C-4AA0-B51E-A930EB1C52F1}" name="name2" dataCellStyle="Normal"/>
     <tableColumn id="6" xr3:uid="{E4F48FEC-C517-4A2D-9E19-3F26D0EECED9}" name="descTerm" dataDxfId="0" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{000852F6-FA93-449A-9A58-91A8EC220656}" name="description" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -445,25 +433,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF1E6EED-0D9B-4163-8683-2C077A96E2AC}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="44.7109375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="117.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="115.8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -476,51 +461,30 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>